<commit_message>
Penambahan Edit Batch & Ubah Casefee
</commit_message>
<xml_diff>
--- a/dokumen/Request IT Payment Received New ITO - May 29.xlsx
+++ b/dokumen/Request IT Payment Received New ITO - May 29.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.0.20\Z Folder\Finance &amp; Accounting\INTERNAL ONLY\OTHERS\REVI\ITO - PAYMENT RECEIVED\Per 29 May 2020\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\medex_casefee\dokumen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BC2D019-DA38-4299-8B93-DE7CC25F70E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{F75066B5-C274-4DC7-B4B9-649D7DEA6B9E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="MEDEX" sheetId="1" r:id="rId1"/>
@@ -1256,7 +1255,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
@@ -1336,7 +1335,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{B78FC9DB-4646-4984-BFC7-0460698CE2AB}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1647,11 +1646,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8F4C867-CC57-43BF-B958-18031AEBB4E5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E159"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="A1:E159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4372,11 +4371,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576FB476-1510-480B-828B-FCECFBBBF4C1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>